<commit_message>
Added readme explainer for run_load_data(), reordered manifest cols
</commit_message>
<xml_diff>
--- a/input/manifest/manifest.xlsx
+++ b/input/manifest/manifest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABaker9\Department of Health and Social Care\Evidence and Analysis - 20240319_consultation_training\consultation_example\input\manifest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthsharedservice.sharepoint.com/sites/sr-ple-ea/analytlead/Statistics and Data Science/Data Science/Products &amp; Projects/20240319_consultation_training/consultation_example/input/manifest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1433A636-A230-4773-9A95-1FD9295C4FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1433A636-A230-4773-9A95-1FD9295C4FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048B52B4-478D-4B09-8186-6CC313C43AD4}"/>
   <bookViews>
-    <workbookView xWindow="32670" yWindow="-2835" windowWidth="20805" windowHeight="12465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30015" yWindow="-3930" windowWidth="16605" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
@@ -266,9 +266,6 @@
     <t>likert</t>
   </si>
   <si>
-    <t>assumed_answer</t>
-  </si>
-  <si>
     <t>yes_no</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>An individual sharing my personal views and experiences</t>
+  </si>
+  <si>
+    <t>assumed_easy</t>
   </si>
 </sst>
 </file>
@@ -607,16 +607,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="18.5546875" customWidth="1"/>
     <col min="3" max="3" width="6.77734375" customWidth="1"/>
-    <col min="4" max="6" width="18.5546875" customWidth="1"/>
-    <col min="7" max="8" width="11.109375" customWidth="1"/>
+    <col min="4" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -636,19 +636,19 @@
         <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -661,8 +661,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>82</v>
+      <c r="G2" t="s">
+        <v>81</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -690,7 +690,7 @@
       <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="F3">
         <v>1</v>
       </c>
       <c r="H3" t="b">
@@ -719,7 +719,7 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="F4">
         <v>2</v>
       </c>
       <c r="H4" t="b">
@@ -748,7 +748,7 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="G5">
+      <c r="F5">
         <v>3</v>
       </c>
       <c r="H5" t="b">
@@ -777,7 +777,7 @@
       <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="F6">
         <v>4</v>
       </c>
       <c r="H6" t="b">
@@ -806,7 +806,7 @@
       <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="F7">
         <v>5</v>
       </c>
       <c r="H7" t="b">
@@ -835,7 +835,7 @@
       <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="F8">
         <v>6</v>
       </c>
       <c r="H8" t="b">
@@ -904,7 +904,7 @@
       <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="F11">
         <v>7</v>
       </c>
       <c r="H11" t="b">
@@ -933,7 +933,7 @@
       <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="G12">
+      <c r="F12">
         <v>8</v>
       </c>
       <c r="H12" t="b">
@@ -962,7 +962,7 @@
       <c r="E13" t="s">
         <v>1</v>
       </c>
-      <c r="G13">
+      <c r="F13">
         <v>9</v>
       </c>
       <c r="H13" t="b">
@@ -991,7 +991,7 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="G14">
+      <c r="F14">
         <v>10</v>
       </c>
       <c r="H14" t="b">
@@ -1020,7 +1020,7 @@
       <c r="E15" t="s">
         <v>1</v>
       </c>
-      <c r="G15">
+      <c r="F15">
         <v>11</v>
       </c>
       <c r="H15" t="b">
@@ -1049,7 +1049,7 @@
       <c r="E16" t="s">
         <v>8</v>
       </c>
-      <c r="G16">
+      <c r="F16">
         <v>12</v>
       </c>
       <c r="H16" t="b">
@@ -1069,7 +1069,7 @@
       <c r="C17">
         <v>16</v>
       </c>
-      <c r="G17">
+      <c r="F17">
         <v>13</v>
       </c>
       <c r="H17" t="b">
@@ -1089,7 +1089,7 @@
       <c r="C18">
         <v>17</v>
       </c>
-      <c r="G18">
+      <c r="F18">
         <v>14</v>
       </c>
       <c r="H18" t="b">
@@ -1109,7 +1109,7 @@
       <c r="C19">
         <v>18</v>
       </c>
-      <c r="G19">
+      <c r="F19">
         <v>15</v>
       </c>
       <c r="H19" t="b">
@@ -1129,7 +1129,7 @@
       <c r="C20">
         <v>19</v>
       </c>
-      <c r="G20">
+      <c r="F20">
         <v>16</v>
       </c>
       <c r="H20" t="b">
@@ -1149,7 +1149,7 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="G21">
+      <c r="F21">
         <v>17</v>
       </c>
       <c r="H21" t="b">
@@ -1169,7 +1169,7 @@
       <c r="C22">
         <v>21</v>
       </c>
-      <c r="G22">
+      <c r="F22">
         <v>18</v>
       </c>
       <c r="H22" t="b">
@@ -1189,7 +1189,7 @@
       <c r="C23">
         <v>22</v>
       </c>
-      <c r="G23">
+      <c r="F23">
         <v>19</v>
       </c>
       <c r="H23" t="b">
@@ -1224,7 +1224,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1306,7 +1306,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1451,7 +1451,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1519,7 +1519,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1587,7 +1587,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1673,16 +1673,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AF14F300012244BA79AC1F66BBF765A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="553212c356cb11e2701639f8ab4feb3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d" xmlns:ns3="7aa07ef2-f4ec-4a8c-98d7-e2e24130d9f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca9dd0b1081054472e26110f86c3e149" ns2:_="" ns3:_="">
     <xsd:import namespace="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
@@ -1893,6 +1883,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1903,16 +1903,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61376B99-AB15-40D0-986B-390EED01ACD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C414CE0E-4A17-4111-A80A-8C2755E90A9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1931,6 +1921,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61376B99-AB15-40D0-986B-390EED01ACD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF8C4B93-8167-42F4-ACC0-30DCA1C69AAD}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added scalable custom mappings
</commit_message>
<xml_diff>
--- a/input/manifest/manifest.xlsx
+++ b/input/manifest/manifest.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthsharedservice.sharepoint.com/sites/sr-ple-ea/analytlead/Statistics and Data Science/Data Science/Products &amp; Projects/20240319_consultation_training/consultation_example/input/manifest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{1433A636-A230-4773-9A95-1FD9295C4FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048B52B4-478D-4B09-8186-6CC313C43AD4}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{1433A636-A230-4773-9A95-1FD9295C4FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44EAF2BA-5068-4F2C-B579-D133CCCE57C0}"/>
   <bookViews>
-    <workbookView xWindow="30015" yWindow="-3930" windowWidth="16605" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
     <sheet name="map_likert" sheetId="10" r:id="rId2"/>
-    <sheet name="map2" sheetId="3" r:id="rId3"/>
-    <sheet name="map4" sheetId="4" r:id="rId4"/>
-    <sheet name="map5" sheetId="5" r:id="rId5"/>
+    <sheet name="map_yesno" sheetId="5" r:id="rId3"/>
+    <sheet name="map2" sheetId="3" r:id="rId4"/>
+    <sheet name="map4" sheetId="4" r:id="rId5"/>
     <sheet name="map6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="87">
   <si>
     <t>col_id</t>
   </si>
@@ -263,12 +263,6 @@
     <t>Please explain your answer_2</t>
   </si>
   <si>
-    <t>likert</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
     <t>final</t>
   </si>
   <si>
@@ -279,6 +273,24 @@
   </si>
   <si>
     <t>assumed_easy</t>
+  </si>
+  <si>
+    <t>custom_map</t>
+  </si>
+  <si>
+    <t>map4</t>
+  </si>
+  <si>
+    <t>map6</t>
+  </si>
+  <si>
+    <t>map_yesno</t>
+  </si>
+  <si>
+    <t>map_likert</t>
+  </si>
+  <si>
+    <t>map2</t>
   </si>
 </sst>
 </file>
@@ -605,9 +617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -619,7 +633,7 @@
     <col min="8" max="8" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -639,19 +653,16 @@
         <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -662,19 +673,13 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -696,14 +701,8 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -725,14 +724,11 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -754,14 +750,8 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -783,14 +773,11 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -812,14 +799,11 @@
       <c r="H7" t="b">
         <v>0</v>
       </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -841,14 +825,11 @@
       <c r="H8" t="b">
         <v>0</v>
       </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -861,14 +842,8 @@
       <c r="H9" t="b">
         <v>0</v>
       </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -881,14 +856,8 @@
       <c r="H10" t="b">
         <v>0</v>
       </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -910,14 +879,11 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -939,14 +905,11 @@
       <c r="H12" t="b">
         <v>0</v>
       </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -968,14 +931,11 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -997,14 +957,8 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1026,14 +980,11 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -1055,14 +1006,8 @@
       <c r="H16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1075,14 +1020,8 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1095,14 +1034,8 @@
       <c r="H18" t="b">
         <v>1</v>
       </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1115,14 +1048,8 @@
       <c r="H19" t="b">
         <v>1</v>
       </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1135,14 +1062,8 @@
       <c r="H20" t="b">
         <v>1</v>
       </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1155,14 +1076,8 @@
       <c r="H21" t="b">
         <v>1</v>
       </c>
-      <c r="I21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1175,14 +1090,8 @@
       <c r="H22" t="b">
         <v>1</v>
       </c>
-      <c r="I22" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1194,12 +1103,6 @@
       </c>
       <c r="H23" t="b">
         <v>1</v>
-      </c>
-      <c r="I23" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1224,7 +1127,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1288,6 +1191,74 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3658DD2B-D51F-4AF4-BCBA-BDEFB4EC50AA}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364A1DD1-CBD0-4A2D-86E4-46401D8F16DD}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1306,7 +1277,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1435,7 +1406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA44D45-E54B-44E9-B390-F232CC7F6E6C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1451,7 +1422,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1474,74 +1445,6 @@
       </c>
       <c r="C3" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3658DD2B-D51F-4AF4-BCBA-BDEFB4EC50AA}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1587,7 +1490,7 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1673,6 +1576,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AF14F300012244BA79AC1F66BBF765A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="553212c356cb11e2701639f8ab4feb3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d" xmlns:ns3="7aa07ef2-f4ec-4a8c-98d7-e2e24130d9f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca9dd0b1081054472e26110f86c3e149" ns2:_="" ns3:_="">
     <xsd:import namespace="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
@@ -1883,16 +1796,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1903,6 +1806,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61376B99-AB15-40D0-986B-390EED01ACD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C414CE0E-4A17-4111-A80A-8C2755E90A9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1921,16 +1834,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61376B99-AB15-40D0-986B-390EED01ACD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9abbd945-6b4f-4b5b-8fd0-36fd6d2dad7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF8C4B93-8167-42F4-ACC0-30DCA1C69AAD}">
   <ds:schemaRefs>

</xml_diff>